<commit_message>
added best friends relationships to datap
</commit_message>
<xml_diff>
--- a/data/seating_data.xlsx
+++ b/data/seating_data.xlsx
@@ -129,8 +129,8 @@
   </sheetPr>
   <dimension ref="A1:BM133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V19" activeCellId="0" sqref="V19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AQ24" activeCellId="0" sqref="AQ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -451,7 +451,7 @@
         <v>100</v>
       </c>
       <c r="AM2" s="2" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="AN2" s="2" t="n">
         <v>0</v>
@@ -487,7 +487,7 @@
         <v>100</v>
       </c>
       <c r="AY2" s="2" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="AZ2" s="2" t="n">
         <v>0</v>
@@ -499,7 +499,7 @@
         <v>0</v>
       </c>
       <c r="BC2" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="BD2" s="2" t="n">
         <v>100</v>
@@ -7629,7 +7629,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>0</v>
@@ -7776,7 +7776,7 @@
         <v>0</v>
       </c>
       <c r="AY39" s="2" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="AZ39" s="2" t="n">
         <v>0</v>
@@ -9993,7 +9993,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C51" s="2" t="n">
         <v>0</v>
@@ -10104,7 +10104,7 @@
         <v>100</v>
       </c>
       <c r="AM51" s="2" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="AN51" s="2" t="n">
         <v>0</v>
@@ -10784,7 +10784,7 @@
         <v>0</v>
       </c>
       <c r="C55" s="2" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D55" s="2" t="n">
         <v>0</v>

</xml_diff>